<commit_message>
- Atualização das estatísticas exploratórias
</commit_message>
<xml_diff>
--- a/Estatisticas/Estatísticas.xlsx
+++ b/Estatisticas/Estatísticas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pontificia Universidade Catolica de Goias\9_periodo\Visão Computacional\N2\Maio\projeto\machine-learning-cifar-10\Estatisticas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD46D93-93FB-4B93-A701-996BB30F507B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA0A635-361B-4465-BB18-254C0596C8D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC257B20-F1DB-4089-8EFD-6FE77D34FEFA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Acurácia</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>fc1000</t>
+  </si>
+  <si>
+    <t>0.9033</t>
   </si>
 </sst>
 </file>
@@ -165,7 +168,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -174,6 +177,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -194,31 +200,7 @@
     <cellStyle name="Título 1" xfId="1" builtinId="16"/>
     <cellStyle name="Título 2" xfId="2" builtinId="17"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -293,77 +275,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF6D0838-2208-4B14-B812-3874D36CF177}" name="Tabela1" displayName="Tabela1" ref="A3:B14" totalsRowShown="0" headerRowDxfId="24" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF6D0838-2208-4B14-B812-3874D36CF177}" name="Tabela1" displayName="Tabela1" ref="A3:B14" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A3:B14" xr:uid="{8E7061DE-B65A-49E3-9FE8-5F70D659E1AB}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{550C2B93-0808-4770-A685-72E74B724D96}" name="Trainamento (%)" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{1F4D165C-E56F-4DA6-8C95-070D37D279E8}" name="Acurácia" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{550C2B93-0808-4770-A685-72E74B724D96}" name="Trainamento (%)" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{1F4D165C-E56F-4DA6-8C95-070D37D279E8}" name="Acurácia" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6F1EBB2C-22A3-4BA0-A2F1-D9FEDDFBF709}" name="Tabela2" displayName="Tabela2" ref="A17:B28" totalsRowShown="0" headerRowDxfId="20" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6F1EBB2C-22A3-4BA0-A2F1-D9FEDDFBF709}" name="Tabela2" displayName="Tabela2" ref="A17:B28" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A17:B28" xr:uid="{2430B19F-6BA0-4DAF-9FAC-053E13BAA007}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{41630CA7-CB2F-4DEE-9813-937741A52AEB}" name="Trainamento (%)" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{01CB1DD0-ED95-4169-865C-2C0CFF4604E7}" name="Acurácia" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{41630CA7-CB2F-4DEE-9813-937741A52AEB}" name="Trainamento (%)" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{01CB1DD0-ED95-4169-865C-2C0CFF4604E7}" name="Acurácia" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D602EE40-61FC-4DDC-AC1D-572BB2CD29E5}" name="Tabela3" displayName="Tabela3" ref="A32:B43" totalsRowShown="0" headerRowDxfId="16" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D602EE40-61FC-4DDC-AC1D-572BB2CD29E5}" name="Tabela3" displayName="Tabela3" ref="A32:B43" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A32:B43" xr:uid="{DA662C2C-4F46-4D9E-8180-B85A584EFA13}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6B3D1347-D012-40EB-A928-58D60199EDD0}" name="Trainamento (%)" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{0D781485-0DB4-4951-B87A-36787B72B5D6}" name="Acurácia" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{6B3D1347-D012-40EB-A928-58D60199EDD0}" name="Trainamento (%)" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{0D781485-0DB4-4951-B87A-36787B72B5D6}" name="Acurácia" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{88C35718-AA2C-4045-8257-D82AB60F669A}" name="Tabela35" displayName="Tabela35" ref="D32:E43" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{88C35718-AA2C-4045-8257-D82AB60F669A}" name="Tabela35" displayName="Tabela35" ref="D32:E43" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="D32:E43" xr:uid="{CA356BAD-7889-4783-ABD5-139DADB57D28}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{18A2E71F-49D6-4076-B992-2B48CA819497}" name="Trainamento (%)" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{C71FEC08-AE0F-44FA-8DF6-5603D824DD8B}" name="Acurácia" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{18A2E71F-49D6-4076-B992-2B48CA819497}" name="Trainamento (%)" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{C71FEC08-AE0F-44FA-8DF6-5603D824DD8B}" name="Acurácia" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4ECBDF73-54FD-4C73-9DE3-ACBED1C75A9A}" name="Tabela37" displayName="Tabela37" ref="A48:B59" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4ECBDF73-54FD-4C73-9DE3-ACBED1C75A9A}" name="Tabela37" displayName="Tabela37" ref="A48:B59" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A48:B59" xr:uid="{E4766CE1-586C-41B3-9D23-D955FDC26EB2}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{61285175-6913-4178-8FAA-CBF30FFDB1B7}" name="Trainamento (%)" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{473A572D-8085-46B1-995A-058424DC4BF2}" name="Acurácia" dataDxfId="8"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6AA93009-3E58-423D-AD30-6F830706B88C}" name="Tabela378" displayName="Tabela378" ref="D48:E59" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="D48:E59" xr:uid="{F8B5D57F-7217-4882-B2F6-AEC5E2D86426}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{9D7A0F5F-4357-458E-8C6D-5B6FEB26D667}" name="Trainamento (%)" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{432506C7-4163-4742-95EE-DADB44BCD56A}" name="Acurácia" dataDxfId="4"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E2F54938-CFD1-41A2-90EB-A522E493E808}" name="Tabela379" displayName="Tabela379" ref="G48:H59" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="G48:H59" xr:uid="{E932822E-4144-4D4C-956C-A83CE5905681}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{70CAA335-8E4B-4489-A04F-B11E86C0EDC6}" name="Trainamento (%)" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{CE664B19-633D-4D47-9CAE-1C6C6A72A497}" name="Acurácia" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{61285175-6913-4178-8FAA-CBF30FFDB1B7}" name="Trainamento (%)" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{473A572D-8085-46B1-995A-058424DC4BF2}" name="Acurácia" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -668,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93AEF4A8-00F8-4AF2-9B0A-84C5C68DEBEF}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,22 +643,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -788,10 +748,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="7"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -861,24 +821,24 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="D30" s="5" t="s">
+      <c r="B30" s="6"/>
+      <c r="D30" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="5"/>
+      <c r="E30" s="6"/>
     </row>
     <row r="31" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="D31" s="6" t="s">
+      <c r="B31" s="7"/>
+      <c r="D31" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="6"/>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
@@ -1009,44 +969,28 @@
       <c r="E43" s="4"/>
     </row>
     <row r="45" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
     </row>
     <row r="46" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B46" s="5"/>
-      <c r="D46" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E46" s="5"/>
-      <c r="G46" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H46" s="5"/>
+      <c r="B46" s="6"/>
     </row>
     <row r="47" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B47" s="6"/>
-      <c r="D47" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E47" s="6"/>
-      <c r="G47" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H47" s="6"/>
+      <c r="B47" s="7"/>
     </row>
     <row r="48" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
@@ -1055,183 +999,81 @@
       <c r="B48" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H48" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>1</v>
       </c>
       <c r="B49" s="4"/>
-      <c r="D49" s="4">
-        <v>1</v>
-      </c>
-      <c r="E49" s="4"/>
-      <c r="G49" s="4">
-        <v>1</v>
-      </c>
-      <c r="H49" s="4"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>10</v>
       </c>
       <c r="B50" s="3"/>
-      <c r="D50" s="4">
-        <v>10</v>
-      </c>
-      <c r="E50" s="3"/>
-      <c r="G50" s="4">
-        <v>10</v>
-      </c>
-      <c r="H50" s="3"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>20</v>
       </c>
       <c r="B51" s="4"/>
-      <c r="D51" s="4">
-        <v>20</v>
-      </c>
-      <c r="E51" s="4"/>
-      <c r="G51" s="4">
-        <v>20</v>
-      </c>
-      <c r="H51" s="4"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>30</v>
       </c>
       <c r="B52" s="4"/>
-      <c r="D52" s="4">
-        <v>30</v>
-      </c>
-      <c r="E52" s="4"/>
-      <c r="G52" s="4">
-        <v>30</v>
-      </c>
-      <c r="H52" s="4"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>40</v>
       </c>
       <c r="B53" s="4"/>
-      <c r="D53" s="4">
-        <v>40</v>
-      </c>
-      <c r="E53" s="4"/>
-      <c r="G53" s="4">
-        <v>40</v>
-      </c>
-      <c r="H53" s="4"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>50</v>
       </c>
       <c r="B54" s="4"/>
-      <c r="D54" s="4">
-        <v>50</v>
-      </c>
-      <c r="E54" s="4"/>
-      <c r="G54" s="4">
-        <v>50</v>
-      </c>
-      <c r="H54" s="4"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>60</v>
       </c>
       <c r="B55" s="4"/>
-      <c r="D55" s="4">
-        <v>60</v>
-      </c>
-      <c r="E55" s="4"/>
-      <c r="G55" s="4">
-        <v>60</v>
-      </c>
-      <c r="H55" s="4"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>70</v>
       </c>
       <c r="B56" s="4"/>
-      <c r="D56" s="4">
-        <v>70</v>
-      </c>
-      <c r="E56" s="4"/>
-      <c r="G56" s="4">
-        <v>70</v>
-      </c>
-      <c r="H56" s="4"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>80</v>
       </c>
-      <c r="B57" s="4"/>
-      <c r="D57" s="4">
-        <v>80</v>
-      </c>
-      <c r="E57" s="4"/>
-      <c r="G57" s="4">
-        <v>80</v>
-      </c>
-      <c r="H57" s="4"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>90</v>
       </c>
       <c r="B58" s="4"/>
-      <c r="D58" s="4">
-        <v>90</v>
-      </c>
-      <c r="E58" s="4"/>
-      <c r="G58" s="4">
-        <v>90</v>
-      </c>
-      <c r="H58" s="4"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>99</v>
       </c>
       <c r="B59" s="4"/>
-      <c r="D59" s="4">
-        <v>99</v>
-      </c>
-      <c r="E59" s="4"/>
-      <c r="G59" s="4">
-        <v>99</v>
-      </c>
-      <c r="H59" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G47:H47"/>
+  <mergeCells count="10">
     <mergeCell ref="A45:H45"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A31:B31"/>
@@ -1241,14 +1083,12 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
-  <tableParts count="7">
+  <tableParts count="5">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
-    <tablePart r:id="rId7"/>
-    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>